<commit_message>
feat(PYME-4265): add column subscription id in justifications control
</commit_message>
<xml_diff>
--- a/reports/european_funds_justifications_control/templates/xlsx/template.xlsx
+++ b/reports/european_funds_justifications_control/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/european_funds_justifications_control/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B973C16-FA61-4E48-AC4A-D7F725B2E1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Request ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Domain</t>
+  </si>
+  <si>
+    <t>Subscription ID</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -423,12 +426,13 @@
     <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5" customWidth="1"/>
-    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,23 +458,26 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat/pyme 4265 add new column in report (#23)
* feat(PYME-4265): Add subscription id in excel

* Revert "feat(PYME-4265): Add subscription id in excel"

This reverts commit d920faaf007ab035dfb3d6a7884faeb4dda07717.

* feat(PYME-4265): add column subscription id in justifications control

* merge main
</commit_message>
<xml_diff>
--- a/reports/european_funds_justifications_control/templates/xlsx/template.xlsx
+++ b/reports/european_funds_justifications_control/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgelg/git/yssb-devi-reports/reports/european_funds_requests/templates/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cx02538/Telefonica/yssb-devi-reports/reports/european_funds_justifications_control/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCADA8F-E8A3-3840-BAA1-41FA287669E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B973C16-FA61-4E48-AC4A-D7F725B2E1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Request ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Domain</t>
+  </si>
+  <si>
+    <t>Subscription ID</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -423,12 +426,13 @@
     <col min="5" max="6" width="17.5" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5" customWidth="1"/>
-    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,23 +458,26 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
+  <autoFilter ref="A1:N1" xr:uid="{4B4C567F-19CC-43F3-A784-B79D65DF0209}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>